<commit_message>
Updated format and added link
</commit_message>
<xml_diff>
--- a/2019_Outlook/News Aggregate.xlsx
+++ b/2019_Outlook/News Aggregate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10123"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robro\Documents\GitHub\MacIC_Macro\2019_Outlook\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lucaskrenn/GitRepos/MacIC_Macro/2019_Outlook/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D147DDA2-C9E7-4BE5-9ED9-B29B4AF0436E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E3EED80A-91A5-7747-85B2-DA836B84FB04}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6850" xr2:uid="{65BEA301-8910-4632-9288-F51569C5785C}"/>
+    <workbookView xWindow="2220" yWindow="-26860" windowWidth="33600" windowHeight="20520" xr2:uid="{65BEA301-8910-4632-9288-F51569C5785C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="13">
   <si>
     <t>Venezuela</t>
   </si>
@@ -58,13 +57,25 @@
   </si>
   <si>
     <t>Canada China Relations</t>
+  </si>
+  <si>
+    <t>Trudeau ousted Canada's ambassador to China amid claims that the Huawei CFO would have a "good case" against extradition</t>
+  </si>
+  <si>
+    <t>https://www.bloomberg.com/news/articles/2019-01-26/trudeau-s-china-envoy-resigns-after-comments-about-huawei-case?srnd=premium-canada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trudeau is taking the extradition seriously </t>
+  </si>
+  <si>
+    <t>Outlook 2019 MacIC Macro</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -72,16 +83,47 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)_x0000_"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9C0403"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -89,13 +131,158 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -104,6 +291,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF9C0403"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -412,123 +604,173 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F54727F-3B2F-4024-9653-C039CB24AC77}">
-  <dimension ref="B5:AD6"/>
+  <dimension ref="A1:Y7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="22.08984375" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" style="5"/>
+    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.83203125" style="5"/>
+    <col min="7" max="7" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.83203125" style="5"/>
+    <col min="12" max="12" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="31.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.5" customWidth="1"/>
+    <col min="15" max="15" width="33.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.83203125" style="5"/>
+    <col min="17" max="17" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.83203125" style="5"/>
+    <col min="22" max="22" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="16384" width="8.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:30" x14ac:dyDescent="0.35">
-      <c r="B5" s="1" t="s">
+    <row r="1" spans="1:25" s="4" customFormat="1">
+      <c r="A1" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="14"/>
+    </row>
+    <row r="2" spans="1:25" s="4" customFormat="1" ht="16" thickBot="1">
+      <c r="A2" s="15"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="17"/>
+    </row>
+    <row r="3" spans="1:25" s="4" customFormat="1"/>
+    <row r="4" spans="1:25" s="4" customFormat="1" ht="16" thickBot="1"/>
+    <row r="5" spans="1:25" ht="16" thickBot="1">
+      <c r="B5" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="H5" s="1" t="s">
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="G5" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="N5" s="1" t="s">
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="L5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="O5" s="1"/>
-      <c r="P5" s="1"/>
-      <c r="Q5" s="1"/>
-      <c r="R5" s="1"/>
-      <c r="T5" s="1" t="s">
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
+      <c r="O5" s="8"/>
+      <c r="Q5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="U5" s="1"/>
-      <c r="V5" s="1"/>
-      <c r="W5" s="1"/>
-      <c r="X5" s="1"/>
-      <c r="Z5" s="1" t="s">
+      <c r="R5" s="8"/>
+      <c r="S5" s="8"/>
+      <c r="T5" s="8"/>
+      <c r="V5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="AA5" s="1"/>
-      <c r="AB5" s="1"/>
-      <c r="AC5" s="1"/>
-      <c r="AD5" s="1"/>
+      <c r="W5" s="8"/>
+      <c r="X5" s="8"/>
+      <c r="Y5" s="8"/>
     </row>
-    <row r="6" spans="2:30" x14ac:dyDescent="0.35">
-      <c r="B6" t="s">
+    <row r="6" spans="1:25">
+      <c r="B6" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="H6" t="s">
+      <c r="G6" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="I6" t="s">
+      <c r="H6" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="J6" t="s">
+      <c r="I6" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="K6" t="s">
+      <c r="J6" s="12" t="s">
         <v>4</v>
       </c>
+      <c r="L6" t="s">
+        <v>1</v>
+      </c>
+      <c r="M6" t="s">
+        <v>2</v>
+      </c>
       <c r="N6" t="s">
+        <v>3</v>
+      </c>
+      <c r="O6" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q6" t="s">
         <v>1</v>
       </c>
-      <c r="O6" t="s">
+      <c r="R6" t="s">
         <v>2</v>
       </c>
-      <c r="P6" t="s">
+      <c r="S6" t="s">
         <v>3</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="T6" t="s">
         <v>4</v>
       </c>
-      <c r="T6" t="s">
+      <c r="V6" t="s">
         <v>1</v>
       </c>
-      <c r="U6" t="s">
+      <c r="W6" t="s">
         <v>2</v>
       </c>
-      <c r="V6" t="s">
+      <c r="X6" t="s">
         <v>3</v>
       </c>
-      <c r="W6" t="s">
+      <c r="Y6" t="s">
         <v>4</v>
       </c>
-      <c r="Z6" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA6" t="s">
-        <v>2</v>
-      </c>
-      <c r="AB6" t="s">
-        <v>3</v>
-      </c>
-      <c r="AC6" t="s">
-        <v>4</v>
+    </row>
+    <row r="7" spans="1:25" ht="64">
+      <c r="L7" s="1">
+        <v>43493</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="H5:L5"/>
-    <mergeCell ref="N5:R5"/>
-    <mergeCell ref="T5:X5"/>
-    <mergeCell ref="Z5:AD5"/>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>